<commit_message>
Edicion en documentos de pruebas
</commit_message>
<xml_diff>
--- a/0. Analisis/REQUERIMIENTOS/Maqueta_Dev.xlsx
+++ b/0. Analisis/REQUERIMIENTOS/Maqueta_Dev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ambiente\Documents\GitHub\WebWuky\0. Analisis\REQUERIMIENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C87A21F-DA02-439A-B2D2-1217204644C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4937C59-D9F6-4B05-AA32-D6BD530458E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0EC3DF0-8C94-4ABC-AC0A-0CA136EB6599}"/>
   </bookViews>
@@ -909,8 +909,8 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>